<commit_message>
algunos arreglos en las diapos
</commit_message>
<xml_diff>
--- a/Trabajo Practico/Presentacion/grafs.xlsx
+++ b/Trabajo Practico/Presentacion/grafs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="11535" windowHeight="5580"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="9870" windowHeight="3735"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,8 @@
   <definedNames>
     <definedName name="empleados" localSheetId="0">Hoja1!$B$2:$C$10</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
+  <oleSize ref="B1:C10"/>
 </workbook>
 </file>
 
@@ -86,9 +87,31 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="es-AR"/>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR"/>
+              <a:t>Cantidad</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-AR" baseline="0"/>
+              <a:t> de empleados por año</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -181,25 +204,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="66458752"/>
-        <c:axId val="66460288"/>
+        <c:axId val="51745152"/>
+        <c:axId val="51746688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="66458752"/>
+        <c:axId val="51745152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66460288"/>
+        <c:crossAx val="51746688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66460288"/>
+        <c:axId val="51746688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -207,7 +230,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66458752"/>
+        <c:crossAx val="51745152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -216,7 +239,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -548,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>